<commit_message>
revised: 2020/4/11 data added.
</commit_message>
<xml_diff>
--- a/infected-person-per-generation.xlsx
+++ b/infected-person-per-generation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F29B072-6C36-4481-B6AD-EA5A6D88B2BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEE14F9-EBDE-4144-B66D-6E964E61B01A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-130" yWindow="480" windowWidth="25290" windowHeight="9800" xr2:uid="{580EEFA4-BA17-4328-B77F-653AAFB804FB}"/>
+    <workbookView xWindow="3980" yWindow="1070" windowWidth="12110" windowHeight="12420" xr2:uid="{580EEFA4-BA17-4328-B77F-653AAFB804FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Age-Day" sheetId="1" r:id="rId1"/>
@@ -902,6 +902,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1391,6 +1394,9 @@
                       </c:pt>
                       <c:pt idx="70">
                         <c:v>43931</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>43932</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1917,6 +1923,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2651,6 +2660,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -3140,6 +3152,9 @@
                       </c:pt>
                       <c:pt idx="70">
                         <c:v>43931</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>43932</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3637,6 +3652,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -4342,6 +4360,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -5047,6 +5068,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -5752,6 +5776,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -6457,6 +6484,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -7162,6 +7192,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -7867,6 +7900,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -8571,6 +8607,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9277,6 +9316,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -9762,6 +9804,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -10237,6 +10282,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10722,6 +10770,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11203,6 +11254,9 @@
                       </c:pt>
                       <c:pt idx="70">
                         <c:v>43931</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>43932</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -11481,12 +11535,15 @@
                       <c:pt idx="70">
                         <c:v>43931</c:v>
                       </c:pt>
+                      <c:pt idx="71">
+                        <c:v>43932</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
                         <c16:filteredLitCache>
                           <c:numCache>
@@ -11507,7 +11564,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000013-80FC-44FE-B82E-6381CAE7E4B9}"/>
                   </c:ext>
@@ -11749,12 +11806,15 @@
                       <c:pt idx="70">
                         <c:v>43931</c:v>
                       </c:pt>
+                      <c:pt idx="71">
+                        <c:v>43932</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
                         <c16:filteredLitCache>
                           <c:numCache>
@@ -11775,7 +11835,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-80FC-44FE-B82E-6381CAE7E4B9}"/>
                   </c:ext>
@@ -12026,12 +12086,15 @@
                       <c:pt idx="70">
                         <c:v>43931</c:v>
                       </c:pt>
+                      <c:pt idx="71">
+                        <c:v>43932</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
                         <c16:filteredLitCache>
                           <c:numCache>
@@ -12052,7 +12115,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000F-80FC-44FE-B82E-6381CAE7E4B9}"/>
                   </c:ext>
@@ -12493,6 +12556,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13198,6 +13264,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13718,6 +13787,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3F86-432E-8D82-DFE7A8EDB5A1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -13733,6 +13807,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-3F86-432E-8D82-DFE7A8EDB5A1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -13748,6 +13827,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-3F86-432E-8D82-DFE7A8EDB5A1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -13763,6 +13847,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-3F86-432E-8D82-DFE7A8EDB5A1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -13778,6 +13867,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-3F86-432E-8D82-DFE7A8EDB5A1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -13793,6 +13887,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-3F86-432E-8D82-DFE7A8EDB5A1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -13810,6 +13909,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-3F86-432E-8D82-DFE7A8EDB5A1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -13827,6 +13931,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-3F86-432E-8D82-DFE7A8EDB5A1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -13844,6 +13953,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-3F86-432E-8D82-DFE7A8EDB5A1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -13861,6 +13975,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-3F86-432E-8D82-DFE7A8EDB5A1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -13878,6 +13997,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-3F86-432E-8D82-DFE7A8EDB5A1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -14423,6 +14547,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -14648,6 +14775,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>1.2900717003421454</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.382219678938013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15131,6 +15261,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -15356,6 +15489,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>2.3399979595217792</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.8079975514261348</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15839,6 +15975,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -16064,6 +16203,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>16.363088317616157</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>18.315176046735278</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16547,6 +16689,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -16772,6 +16917,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>18.114319572016313</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>20.037068576867206</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17255,6 +17403,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -17480,6 +17631,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>13.565223538976818</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>15.641984145921153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17963,6 +18117,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -18188,6 +18345,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>13.065914098227109</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>15.446343792236098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18671,6 +18831,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -18896,6 +19059,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>12.717828537949858</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>14.003901086731306</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19389,6 +19555,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -19869,6 +20038,9 @@
                       </c:pt>
                       <c:pt idx="70">
                         <c:v>43931</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>43932</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -20338,6 +20510,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -20563,6 +20738,9 @@
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>11.513280288000495</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>12.145106645268815</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21046,6 +21224,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -21270,6 +21451,9 @@
                   <c:v>8.3861011013328888</c:v>
                 </c:pt>
                 <c:pt idx="69">
+                  <c:v>9.0119295417308667</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>9.0119295417308667</c:v>
                 </c:pt>
               </c:numCache>
@@ -21754,6 +21938,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -21978,6 +22165,9 @@
                   <c:v>9.407962456695703</c:v>
                 </c:pt>
                 <c:pt idx="69">
+                  <c:v>9.9613720129719194</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>9.9613720129719194</c:v>
                 </c:pt>
               </c:numCache>
@@ -22491,6 +22681,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -22980,6 +23173,9 @@
                       </c:pt>
                       <c:pt idx="70">
                         <c:v>43931</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>43932</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -23507,6 +23703,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -23996,6 +24195,9 @@
                       </c:pt>
                       <c:pt idx="70">
                         <c:v>43931</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>43932</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -24522,6 +24724,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -25011,6 +25216,9 @@
                       </c:pt>
                       <c:pt idx="70">
                         <c:v>43931</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>43932</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -25537,6 +25745,9 @@
                 <c:pt idx="70">
                   <c:v>43931</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -26026,6 +26237,9 @@
                       </c:pt>
                       <c:pt idx="70">
                         <c:v>43931</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>43932</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -26551,6 +26765,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>43931</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -51326,11 +51543,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F35F8AD-834A-4135-8E1A-DF5E8F89D541}">
-  <dimension ref="A1:Y72"/>
+  <dimension ref="A1:Y73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V71" sqref="V71"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -53178,7 +53395,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2">
-        <f t="shared" ref="A41:A72" si="2">A40+1</f>
+        <f t="shared" ref="A41:A73" si="2">A40+1</f>
         <v>43900</v>
       </c>
       <c r="B41">
@@ -54521,6 +54738,48 @@
       </c>
       <c r="M72">
         <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="2">
+        <f t="shared" si="2"/>
+        <v>43932</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>34</v>
+      </c>
+      <c r="E73">
+        <v>38</v>
+      </c>
+      <c r="F73">
+        <v>47</v>
+      </c>
+      <c r="G73">
+        <v>45</v>
+      </c>
+      <c r="H73">
+        <v>18</v>
+      </c>
+      <c r="I73">
+        <v>9</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -54533,11 +54792,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B300A435-2B3C-4E24-8831-5A6311C2EBF5}">
-  <dimension ref="A1:AK72"/>
+  <dimension ref="A1:AK73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
+      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -55443,7 +55702,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
-        <f t="shared" ref="A9:A72" si="13">A8+1</f>
+        <f t="shared" ref="A9:A73" si="13">A8+1</f>
         <v>43868</v>
       </c>
       <c r="B9">
@@ -62036,6 +62295,108 @@
       </c>
       <c r="Y72" s="3">
         <f t="shared" ref="Y72" si="49">Y71+X72</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="2">
+        <f t="shared" si="13"/>
+        <v>43932</v>
+      </c>
+      <c r="B73">
+        <f>'Age-Day'!B73</f>
+        <v>1</v>
+      </c>
+      <c r="C73" s="3">
+        <f t="shared" ref="C73" si="50">C72+B73</f>
+        <v>15</v>
+      </c>
+      <c r="D73">
+        <f>'Age-Day'!C73</f>
+        <v>5</v>
+      </c>
+      <c r="E73" s="3">
+        <f t="shared" ref="E73" si="51">E72+D73</f>
+        <v>30</v>
+      </c>
+      <c r="F73">
+        <f>'Age-Day'!D73</f>
+        <v>34</v>
+      </c>
+      <c r="G73" s="3">
+        <f t="shared" ref="G73" si="52">G72+F73</f>
+        <v>319</v>
+      </c>
+      <c r="H73">
+        <f>'Age-Day'!E73</f>
+        <v>38</v>
+      </c>
+      <c r="I73" s="3">
+        <f t="shared" ref="I73" si="53">I72+H73</f>
+        <v>396</v>
+      </c>
+      <c r="J73">
+        <f>'Age-Day'!F73</f>
+        <v>47</v>
+      </c>
+      <c r="K73" s="3">
+        <f t="shared" ref="K73" si="54">K72+J73</f>
+        <v>354</v>
+      </c>
+      <c r="L73">
+        <f>'Age-Day'!G73</f>
+        <v>45</v>
+      </c>
+      <c r="M73" s="3">
+        <f t="shared" ref="M73" si="55">M72+L73</f>
+        <v>292</v>
+      </c>
+      <c r="N73">
+        <f>'Age-Day'!H73</f>
+        <v>18</v>
+      </c>
+      <c r="O73" s="3">
+        <f t="shared" ref="O73" si="56">O72+N73</f>
+        <v>196</v>
+      </c>
+      <c r="P73">
+        <f>'Age-Day'!I73</f>
+        <v>9</v>
+      </c>
+      <c r="Q73" s="3">
+        <f t="shared" ref="Q73" si="57">Q72+P73</f>
+        <v>173</v>
+      </c>
+      <c r="R73">
+        <f>'Age-Day'!J73</f>
+        <v>0</v>
+      </c>
+      <c r="S73" s="3">
+        <f t="shared" ref="S73" si="58">S72+R73</f>
+        <v>72</v>
+      </c>
+      <c r="T73">
+        <f>'Age-Day'!K73</f>
+        <v>0</v>
+      </c>
+      <c r="U73" s="3">
+        <f t="shared" ref="U73" si="59">U72+T73</f>
+        <v>18</v>
+      </c>
+      <c r="V73">
+        <f>'Age-Day'!L73</f>
+        <v>0</v>
+      </c>
+      <c r="W73" s="3">
+        <f t="shared" ref="W73" si="60">W72+V73</f>
+        <v>0</v>
+      </c>
+      <c r="X73">
+        <f>'Age-Day'!M73</f>
+        <v>0</v>
+      </c>
+      <c r="Y73" s="3">
+        <f t="shared" ref="Y73" si="61">Y72+X73</f>
         <v>14</v>
       </c>
     </row>
@@ -62049,11 +62410,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{156A320C-30E6-4277-A9A2-5F5B18FB0A95}">
-  <dimension ref="A1:BA72"/>
+  <dimension ref="A1:BA73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F74" sqref="F74"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -63380,7 +63741,7 @@
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
-        <f t="shared" ref="A9:A72" si="24">A8+1</f>
+        <f t="shared" ref="A9:A73" si="24">A8+1</f>
         <v>43868</v>
       </c>
       <c r="B9">
@@ -71605,7 +71966,7 @@
         <v>8</v>
       </c>
       <c r="D66" s="5">
-        <f t="shared" ref="D66:D72" si="35">($C66/1085211)*100000</f>
+        <f t="shared" ref="D66:D73" si="35">($C66/1085211)*100000</f>
         <v>0.73718382876694022</v>
       </c>
       <c r="E66">
@@ -71617,7 +71978,7 @@
         <v>16</v>
       </c>
       <c r="G66" s="5">
-        <f t="shared" ref="G66:G72" si="36">($F66/1068377)*100000</f>
+        <f t="shared" ref="G66:G73" si="36">($F66/1068377)*100000</f>
         <v>1.4975986940939388</v>
       </c>
       <c r="H66">
@@ -71629,7 +71990,7 @@
         <v>124</v>
       </c>
       <c r="J66" s="5">
-        <f t="shared" ref="J66:J72" si="37">($I66/1741725)*100000</f>
+        <f t="shared" ref="J66:J73" si="37">($I66/1741725)*100000</f>
         <v>7.1193787767873813</v>
       </c>
       <c r="K66">
@@ -71641,7 +72002,7 @@
         <v>167</v>
       </c>
       <c r="M66" s="5">
-        <f t="shared" ref="M66:M72" si="38">($L66/1976337)*100000</f>
+        <f t="shared" ref="M66:M73" si="38">($L66/1976337)*100000</f>
         <v>8.4499758897394521</v>
       </c>
       <c r="N66">
@@ -71653,7 +72014,7 @@
         <v>171</v>
       </c>
       <c r="P66" s="5">
-        <f t="shared" ref="P66:P72" si="39">($O66/2263140)*100000</f>
+        <f t="shared" ref="P66:P73" si="39">($O66/2263140)*100000</f>
         <v>7.555873697605981</v>
       </c>
       <c r="Q66">
@@ -71665,7 +72026,7 @@
         <v>122</v>
       </c>
       <c r="S66" s="5">
-        <f t="shared" ref="S66:S72" si="40">($R66/1890415)*100000</f>
+        <f t="shared" ref="S66:S73" si="40">($R66/1890415)*100000</f>
         <v>6.4536093926465883</v>
       </c>
       <c r="T66">
@@ -71677,7 +72038,7 @@
         <v>94</v>
       </c>
       <c r="V66" s="5">
-        <f t="shared" ref="V66:V72" si="41">($U66/1399610)*100000</f>
+        <f t="shared" ref="V66:V73" si="41">($U66/1399610)*100000</f>
         <v>6.7161566436364408</v>
       </c>
       <c r="W66">
@@ -71689,7 +72050,7 @@
         <v>107</v>
       </c>
       <c r="Y66" s="5">
-        <f t="shared" ref="Y66:Y72" si="42">($X66/1424442)*100000</f>
+        <f t="shared" ref="Y66:Y73" si="42">($X66/1424442)*100000</f>
         <v>7.5117133586344682</v>
       </c>
       <c r="Z66">
@@ -71701,7 +72062,7 @@
         <v>37</v>
       </c>
       <c r="AB66" s="5">
-        <f t="shared" ref="AB66:AB72" si="43">($AA66/798941)*100000</f>
+        <f t="shared" ref="AB66:AB73" si="43">($AA66/798941)*100000</f>
         <v>4.6311304589450284</v>
       </c>
       <c r="AC66">
@@ -71713,7 +72074,7 @@
         <v>12</v>
       </c>
       <c r="AE66" s="5">
-        <f t="shared" ref="AE66:AE72" si="44">($AD66/180698)*100000</f>
+        <f t="shared" ref="AE66:AE73" si="44">($AD66/180698)*100000</f>
         <v>6.6409146753146127</v>
       </c>
       <c r="AF66">
@@ -72582,6 +72943,148 @@
       </c>
       <c r="AI72" s="3">
         <f t="shared" ref="AI72" si="68">AI71+AH72</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:35" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="2">
+        <f t="shared" si="24"/>
+        <v>43932</v>
+      </c>
+      <c r="B73">
+        <f>'Age-Day'!B73</f>
+        <v>1</v>
+      </c>
+      <c r="C73" s="3">
+        <f t="shared" ref="C73" si="69">C72+B73</f>
+        <v>15</v>
+      </c>
+      <c r="D73" s="5">
+        <f t="shared" si="35"/>
+        <v>1.382219678938013</v>
+      </c>
+      <c r="E73">
+        <f>'Age-Day'!C73</f>
+        <v>5</v>
+      </c>
+      <c r="F73" s="3">
+        <f t="shared" ref="F73" si="70">F72+E73</f>
+        <v>30</v>
+      </c>
+      <c r="G73" s="5">
+        <f t="shared" si="36"/>
+        <v>2.8079975514261348</v>
+      </c>
+      <c r="H73">
+        <f>'Age-Day'!D73</f>
+        <v>34</v>
+      </c>
+      <c r="I73" s="3">
+        <f t="shared" ref="I73" si="71">I72+H73</f>
+        <v>319</v>
+      </c>
+      <c r="J73" s="5">
+        <f t="shared" si="37"/>
+        <v>18.315176046735278</v>
+      </c>
+      <c r="K73">
+        <f>'Age-Day'!E73</f>
+        <v>38</v>
+      </c>
+      <c r="L73" s="3">
+        <f t="shared" ref="L73" si="72">L72+K73</f>
+        <v>396</v>
+      </c>
+      <c r="M73" s="5">
+        <f t="shared" si="38"/>
+        <v>20.037068576867206</v>
+      </c>
+      <c r="N73">
+        <f>'Age-Day'!F73</f>
+        <v>47</v>
+      </c>
+      <c r="O73" s="3">
+        <f t="shared" ref="O73" si="73">O72+N73</f>
+        <v>354</v>
+      </c>
+      <c r="P73" s="5">
+        <f t="shared" si="39"/>
+        <v>15.641984145921153</v>
+      </c>
+      <c r="Q73">
+        <f>'Age-Day'!G73</f>
+        <v>45</v>
+      </c>
+      <c r="R73" s="3">
+        <f t="shared" ref="R73" si="74">R72+Q73</f>
+        <v>292</v>
+      </c>
+      <c r="S73" s="5">
+        <f t="shared" si="40"/>
+        <v>15.446343792236098</v>
+      </c>
+      <c r="T73">
+        <f>'Age-Day'!H73</f>
+        <v>18</v>
+      </c>
+      <c r="U73" s="3">
+        <f t="shared" ref="U73" si="75">U72+T73</f>
+        <v>196</v>
+      </c>
+      <c r="V73" s="5">
+        <f t="shared" si="41"/>
+        <v>14.003901086731306</v>
+      </c>
+      <c r="W73">
+        <f>'Age-Day'!I73</f>
+        <v>9</v>
+      </c>
+      <c r="X73" s="3">
+        <f t="shared" ref="X73" si="76">X72+W73</f>
+        <v>173</v>
+      </c>
+      <c r="Y73" s="5">
+        <f t="shared" si="42"/>
+        <v>12.145106645268815</v>
+      </c>
+      <c r="Z73">
+        <f>'Age-Day'!J73</f>
+        <v>0</v>
+      </c>
+      <c r="AA73" s="3">
+        <f t="shared" ref="AA73" si="77">AA72+Z73</f>
+        <v>72</v>
+      </c>
+      <c r="AB73" s="5">
+        <f t="shared" si="43"/>
+        <v>9.0119295417308667</v>
+      </c>
+      <c r="AC73">
+        <f>'Age-Day'!K73</f>
+        <v>0</v>
+      </c>
+      <c r="AD73" s="3">
+        <f t="shared" ref="AD73" si="78">AD72+AC73</f>
+        <v>18</v>
+      </c>
+      <c r="AE73" s="5">
+        <f t="shared" si="44"/>
+        <v>9.9613720129719194</v>
+      </c>
+      <c r="AF73">
+        <f>'Age-Day'!L73</f>
+        <v>0</v>
+      </c>
+      <c r="AG73" s="3">
+        <f t="shared" ref="AG73" si="79">AG72+AF73</f>
+        <v>0</v>
+      </c>
+      <c r="AH73">
+        <f>'Age-Day'!M73</f>
+        <v>0</v>
+      </c>
+      <c r="AI73" s="3">
+        <f t="shared" ref="AI73" si="80">AI72+AH73</f>
         <v>14</v>
       </c>
     </row>

</xml_diff>